<commit_message>
Show skill is working nicely - last commit before adding voice only
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="29">
   <si>
     <t>Launch</t>
   </si>
@@ -102,12 +102,6 @@
   </si>
   <si>
     <t>Champion</t>
-  </si>
-  <si>
-    <t>Prompted me with which animals did you see</t>
-  </si>
-  <si>
-    <t>no reprompt</t>
   </si>
   <si>
     <t>Level 6</t>
@@ -115,6 +109,12 @@
   <si>
     <t>Question Mark
 (no cheat)</t>
+  </si>
+  <si>
+    <t>no reprompt? - maybe only a problem after the 1st game you play</t>
+  </si>
+  <si>
+    <t>I've seen this work correctly, give the wrong prompt, and give no prompt</t>
   </si>
 </sst>
 </file>
@@ -167,7 +167,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF0000"/>
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -193,9 +193,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -204,6 +201,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -485,8 +485,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -495,7 +495,7 @@
     <col min="3" max="3" width="26.5" customWidth="1"/>
     <col min="4" max="4" width="26.1640625" customWidth="1"/>
     <col min="5" max="5" width="21.5" customWidth="1"/>
-    <col min="6" max="6" width="21.83203125" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.2">
@@ -531,7 +531,7 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="7"/>
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
@@ -567,7 +567,7 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="5"/>
+      <c r="E4" s="4"/>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -583,7 +583,7 @@
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="5"/>
+      <c r="E5" s="4"/>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -601,12 +601,12 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="7"/>
-      <c r="J6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="G6" s="6"/>
+      <c r="H6" s="6"/>
+      <c r="I6" s="6"/>
+      <c r="J6" s="6"/>
+    </row>
+    <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
         <v>1</v>
       </c>
@@ -619,14 +619,14 @@
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="8"/>
       <c r="F7" s="2" t="s">
-        <v>26</v>
-      </c>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="7"/>
-      <c r="J7" s="7"/>
+        <v>27</v>
+      </c>
+      <c r="G7" s="6"/>
+      <c r="H7" s="6"/>
+      <c r="I7" s="6"/>
+      <c r="J7" s="6"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -643,10 +643,10 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="7"/>
-      <c r="H8" s="7"/>
-      <c r="I8" s="7"/>
-      <c r="J8" s="7"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="6"/>
+      <c r="I8" s="6"/>
+      <c r="J8" s="6"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -663,10 +663,10 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
+      <c r="G9" s="6"/>
+      <c r="H9" s="6"/>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -683,10 +683,10 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="7"/>
-      <c r="H10" s="7"/>
-      <c r="I10" s="7"/>
-      <c r="J10" s="7"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="6"/>
+      <c r="I10" s="6"/>
+      <c r="J10" s="6"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -703,10 +703,10 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="7"/>
-      <c r="H11" s="7"/>
-      <c r="I11" s="7"/>
-      <c r="J11" s="7"/>
+      <c r="G11" s="6"/>
+      <c r="H11" s="6"/>
+      <c r="I11" s="6"/>
+      <c r="J11" s="6"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -721,12 +721,12 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="5"/>
+      <c r="E12" s="4"/>
       <c r="F12" s="2"/>
-      <c r="G12" s="7"/>
-      <c r="H12" s="7"/>
-      <c r="I12" s="7"/>
-      <c r="J12" s="7"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="6"/>
+      <c r="I12" s="6"/>
+      <c r="J12" s="6"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -741,12 +741,12 @@
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="5"/>
+      <c r="E13" s="4"/>
       <c r="F13" s="2"/>
-      <c r="G13" s="7"/>
-      <c r="H13" s="7"/>
-      <c r="I13" s="7"/>
-      <c r="J13" s="7"/>
+      <c r="G13" s="6"/>
+      <c r="H13" s="6"/>
+      <c r="I13" s="6"/>
+      <c r="J13" s="6"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -763,10 +763,10 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="7"/>
-      <c r="H14" s="7"/>
-      <c r="I14" s="7"/>
-      <c r="J14" s="7"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="6"/>
+      <c r="I14" s="6"/>
+      <c r="J14" s="6"/>
     </row>
     <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -781,16 +781,14 @@
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="4"/>
+      <c r="E15" s="8"/>
       <c r="F15" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="G15" s="5" t="s">
-        <v>26</v>
-      </c>
-      <c r="H15" s="7"/>
-      <c r="I15" s="7"/>
-      <c r="J15" s="7"/>
+        <v>28</v>
+      </c>
+      <c r="G15" s="4"/>
+      <c r="H15" s="6"/>
+      <c r="I15" s="6"/>
+      <c r="J15" s="6"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -807,10 +805,10 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7"/>
-      <c r="J16" s="7"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -827,10 +825,10 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="7"/>
-      <c r="H17" s="7"/>
-      <c r="I17" s="7"/>
-      <c r="J17" s="7"/>
+      <c r="G17" s="6"/>
+      <c r="H17" s="6"/>
+      <c r="I17" s="6"/>
+      <c r="J17" s="6"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -847,10 +845,10 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="7"/>
-      <c r="H18" s="7"/>
-      <c r="I18" s="7"/>
-      <c r="J18" s="7"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="6"/>
+      <c r="I18" s="6"/>
+      <c r="J18" s="6"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -867,10 +865,10 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="7"/>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
+      <c r="G19" s="6"/>
+      <c r="H19" s="6"/>
+      <c r="I19" s="6"/>
+      <c r="J19" s="6"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -885,12 +883,12 @@
       <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="6"/>
+      <c r="E20" s="5"/>
       <c r="F20" s="2"/>
-      <c r="G20" s="7"/>
-      <c r="H20" s="7"/>
-      <c r="I20" s="7"/>
-      <c r="J20" s="7"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="6"/>
+      <c r="I20" s="6"/>
+      <c r="J20" s="6"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -905,7 +903,7 @@
       <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="5"/>
+      <c r="E21" s="4"/>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -990,7 +988,7 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A27" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>20</v>
@@ -1006,10 +1004,10 @@
     </row>
     <row r="28" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A28" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="C28" s="2" t="s">
         <v>21</v>
@@ -1017,12 +1015,12 @@
       <c r="D28" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E28" s="5"/>
+      <c r="E28" s="3"/>
       <c r="F28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>24</v>

</xml_diff>

<commit_message>
working nicely on Echo Show and Dot - first submission
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -12,7 +12,8 @@
     <workbookView xWindow="0" yWindow="460" windowWidth="18180" windowHeight="28340" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Show" sheetId="1" r:id="rId1"/>
+    <sheet name="Dot" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="150000" concurrentCalc="0"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="30">
   <si>
     <t>Launch</t>
   </si>
@@ -115,23 +116,19 @@
   </si>
   <si>
     <t>I've seen this work correctly, give the wrong prompt, and give no prompt</t>
+  </si>
+  <si>
+    <t>enhancement</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -184,9 +181,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -196,11 +193,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -486,7 +480,7 @@
   <dimension ref="A1:J56"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+      <selection activeCell="E20" sqref="E20:E21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -518,7 +512,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -531,12 +525,12 @@
       <c r="D2" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="E2" s="7"/>
+      <c r="E2" s="6"/>
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -567,7 +561,9 @@
       <c r="D4" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E4" s="4"/>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.2">
@@ -583,7 +579,9 @@
       <c r="D5" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E5" s="4"/>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.2">
@@ -601,10 +599,10 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="6"/>
-      <c r="I6" s="6"/>
-      <c r="J6" s="6"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
     </row>
     <row r="7" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="2" t="s">
@@ -619,14 +617,14 @@
       <c r="D7" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E7" s="8"/>
+      <c r="E7" s="7"/>
       <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="6"/>
-      <c r="H7" s="6"/>
-      <c r="I7" s="6"/>
-      <c r="J7" s="6"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="2" t="s">
@@ -643,10 +641,10 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="6"/>
-      <c r="I8" s="6"/>
-      <c r="J8" s="6"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="2" t="s">
@@ -663,10 +661,10 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="6"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="2" t="s">
@@ -683,10 +681,10 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="6"/>
-      <c r="I10" s="6"/>
-      <c r="J10" s="6"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="2" t="s">
@@ -703,10 +701,10 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="6"/>
-      <c r="H11" s="6"/>
-      <c r="I11" s="6"/>
-      <c r="J11" s="6"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="2" t="s">
@@ -721,12 +719,14 @@
       <c r="D12" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E12" s="4"/>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F12" s="2"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="6"/>
-      <c r="I12" s="6"/>
-      <c r="J12" s="6"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="2" t="s">
@@ -741,12 +741,14 @@
       <c r="D13" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E13" s="4"/>
+      <c r="E13" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F13" s="2"/>
-      <c r="G13" s="6"/>
-      <c r="H13" s="6"/>
-      <c r="I13" s="6"/>
-      <c r="J13" s="6"/>
+      <c r="G13" s="5"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="2" t="s">
@@ -763,10 +765,10 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="6"/>
-      <c r="I14" s="6"/>
-      <c r="J14" s="6"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
     </row>
     <row r="15" spans="1:10" ht="32" x14ac:dyDescent="0.2">
       <c r="A15" s="2" t="s">
@@ -781,14 +783,14 @@
       <c r="D15" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="7"/>
       <c r="F15" s="2" t="s">
         <v>28</v>
       </c>
       <c r="G15" s="4"/>
-      <c r="H15" s="6"/>
-      <c r="I15" s="6"/>
-      <c r="J15" s="6"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="2" t="s">
@@ -805,10 +807,10 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="6"/>
-      <c r="I16" s="6"/>
-      <c r="J16" s="6"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A17" s="2" t="s">
@@ -825,10 +827,10 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="6"/>
-      <c r="H17" s="6"/>
-      <c r="I17" s="6"/>
-      <c r="J17" s="6"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A18" s="2" t="s">
@@ -845,10 +847,10 @@
       </c>
       <c r="E18" s="3"/>
       <c r="F18" s="2"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="6"/>
-      <c r="I18" s="6"/>
-      <c r="J18" s="6"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A19" s="2" t="s">
@@ -865,10 +867,10 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="6"/>
-      <c r="H19" s="6"/>
-      <c r="I19" s="6"/>
-      <c r="J19" s="6"/>
+      <c r="G19" s="5"/>
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A20" s="2" t="s">
@@ -883,12 +885,14 @@
       <c r="D20" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E20" s="5"/>
+      <c r="E20" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F20" s="2"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="6"/>
-      <c r="I20" s="6"/>
-      <c r="J20" s="6"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="5"/>
+      <c r="I20" s="5"/>
+      <c r="J20" s="5"/>
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A21" s="2" t="s">
@@ -903,7 +907,9 @@
       <c r="D21" s="2" t="s">
         <v>17</v>
       </c>
-      <c r="E21" s="4"/>
+      <c r="E21" s="4" t="s">
+        <v>29</v>
+      </c>
       <c r="F21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
@@ -1259,4 +1265,736 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:J53"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="2" width="22" customWidth="1"/>
+    <col min="3" max="3" width="26.5" customWidth="1"/>
+    <col min="4" max="4" width="26.1640625" customWidth="1"/>
+    <col min="5" max="5" width="21.5" customWidth="1"/>
+    <col min="6" max="6" width="46" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6"/>
+      <c r="F2" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A3" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E3" s="3"/>
+      <c r="F3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A4" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="2"/>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A5" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F5" s="2"/>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A6" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="5"/>
+      <c r="I6" s="5"/>
+      <c r="J6" s="5"/>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A7" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="5"/>
+      <c r="H7" s="5"/>
+      <c r="I7" s="5"/>
+      <c r="J7" s="5"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="5"/>
+      <c r="I8" s="5"/>
+      <c r="J8" s="5"/>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="5"/>
+      <c r="H9" s="5"/>
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="5"/>
+      <c r="I10" s="5"/>
+      <c r="J10" s="5"/>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F11" s="2"/>
+      <c r="G11" s="5"/>
+      <c r="H11" s="5"/>
+      <c r="I11" s="5"/>
+      <c r="J11" s="5"/>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F12" s="2"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="5"/>
+      <c r="I12" s="5"/>
+      <c r="J12" s="5"/>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="4"/>
+      <c r="H13" s="5"/>
+      <c r="I13" s="5"/>
+      <c r="J13" s="5"/>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="5"/>
+      <c r="I14" s="5"/>
+      <c r="J14" s="5"/>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="5"/>
+      <c r="H15" s="5"/>
+      <c r="I15" s="5"/>
+      <c r="J15" s="5"/>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="5"/>
+      <c r="I16" s="5"/>
+      <c r="J16" s="5"/>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A17" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E17" s="3"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="5"/>
+      <c r="H17" s="5"/>
+      <c r="I17" s="5"/>
+      <c r="J17" s="5"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A18" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F18" s="2"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="5"/>
+      <c r="I18" s="5"/>
+      <c r="J18" s="5"/>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A19" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E19" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="F19" s="2"/>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A20" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E20" s="3"/>
+      <c r="F20" s="2"/>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A21" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E21" s="3"/>
+      <c r="F21" s="2"/>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A22" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E22" s="3"/>
+      <c r="F22" s="2"/>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A23" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E23" s="3"/>
+      <c r="F23" s="2"/>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E24" s="4"/>
+      <c r="F24" s="2"/>
+    </row>
+    <row r="25" spans="1:10" ht="32" x14ac:dyDescent="0.2">
+      <c r="A25" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B25" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="C25" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E25" s="4"/>
+      <c r="F25" s="2"/>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A26" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C26" s="2"/>
+      <c r="D26" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="4"/>
+      <c r="F26" s="2"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A27" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E27" s="3"/>
+      <c r="F27" s="2"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A28" s="2"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+      <c r="D28" s="2"/>
+      <c r="E28" s="2"/>
+      <c r="F28" s="2"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A29" s="2"/>
+      <c r="B29" s="2"/>
+      <c r="C29" s="2"/>
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" s="2"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A30" s="2"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="2"/>
+      <c r="D30" s="2"/>
+      <c r="E30" s="2"/>
+      <c r="F30" s="2"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A31" s="2"/>
+      <c r="B31" s="2"/>
+      <c r="C31" s="2"/>
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" s="2"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.2">
+      <c r="A32" s="2"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="2"/>
+      <c r="D32" s="2"/>
+      <c r="E32" s="2"/>
+      <c r="F32" s="2"/>
+    </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A33" s="2"/>
+      <c r="B33" s="2"/>
+      <c r="C33" s="2"/>
+      <c r="D33" s="2"/>
+      <c r="E33" s="2"/>
+      <c r="F33" s="2"/>
+    </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A34" s="2"/>
+      <c r="B34" s="2"/>
+      <c r="C34" s="2"/>
+      <c r="D34" s="2"/>
+      <c r="E34" s="2"/>
+      <c r="F34" s="2"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A35" s="2"/>
+      <c r="B35" s="2"/>
+      <c r="C35" s="2"/>
+      <c r="D35" s="2"/>
+      <c r="E35" s="2"/>
+      <c r="F35" s="2"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A36" s="2"/>
+      <c r="B36" s="2"/>
+      <c r="C36" s="2"/>
+      <c r="D36" s="2"/>
+      <c r="E36" s="2"/>
+      <c r="F36" s="2"/>
+    </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A37" s="2"/>
+      <c r="B37" s="2"/>
+      <c r="C37" s="2"/>
+      <c r="D37" s="2"/>
+      <c r="E37" s="2"/>
+      <c r="F37" s="2"/>
+    </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A38" s="2"/>
+      <c r="B38" s="2"/>
+      <c r="C38" s="2"/>
+      <c r="D38" s="2"/>
+      <c r="E38" s="2"/>
+      <c r="F38" s="2"/>
+    </row>
+    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A39" s="2"/>
+      <c r="B39" s="2"/>
+      <c r="C39" s="2"/>
+      <c r="D39" s="2"/>
+      <c r="E39" s="2"/>
+      <c r="F39" s="2"/>
+    </row>
+    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A40" s="2"/>
+      <c r="B40" s="2"/>
+      <c r="C40" s="2"/>
+      <c r="D40" s="2"/>
+      <c r="E40" s="2"/>
+      <c r="F40" s="2"/>
+    </row>
+    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A41" s="2"/>
+      <c r="B41" s="2"/>
+      <c r="C41" s="2"/>
+      <c r="D41" s="2"/>
+      <c r="E41" s="2"/>
+      <c r="F41" s="2"/>
+    </row>
+    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A42" s="2"/>
+      <c r="B42" s="2"/>
+      <c r="C42" s="2"/>
+      <c r="D42" s="2"/>
+      <c r="E42" s="2"/>
+      <c r="F42" s="2"/>
+    </row>
+    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A43" s="2"/>
+      <c r="B43" s="2"/>
+      <c r="C43" s="2"/>
+      <c r="D43" s="2"/>
+      <c r="E43" s="2"/>
+      <c r="F43" s="2"/>
+    </row>
+    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A44" s="2"/>
+      <c r="B44" s="2"/>
+      <c r="C44" s="2"/>
+      <c r="D44" s="2"/>
+      <c r="E44" s="2"/>
+      <c r="F44" s="2"/>
+    </row>
+    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A45" s="2"/>
+      <c r="B45" s="2"/>
+      <c r="C45" s="2"/>
+      <c r="D45" s="2"/>
+      <c r="E45" s="2"/>
+      <c r="F45" s="2"/>
+    </row>
+    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A46" s="2"/>
+      <c r="B46" s="2"/>
+      <c r="C46" s="2"/>
+      <c r="D46" s="2"/>
+      <c r="E46" s="2"/>
+      <c r="F46" s="2"/>
+    </row>
+    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A47" s="2"/>
+      <c r="B47" s="2"/>
+      <c r="C47" s="2"/>
+      <c r="D47" s="2"/>
+      <c r="E47" s="2"/>
+      <c r="F47" s="2"/>
+    </row>
+    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A48" s="2"/>
+      <c r="B48" s="2"/>
+      <c r="C48" s="2"/>
+      <c r="D48" s="2"/>
+      <c r="E48" s="2"/>
+      <c r="F48" s="2"/>
+    </row>
+    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A49" s="2"/>
+      <c r="B49" s="2"/>
+      <c r="C49" s="2"/>
+      <c r="D49" s="2"/>
+      <c r="E49" s="2"/>
+      <c r="F49" s="2"/>
+    </row>
+    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A50" s="2"/>
+      <c r="B50" s="2"/>
+      <c r="C50" s="2"/>
+      <c r="D50" s="2"/>
+      <c r="E50" s="2"/>
+      <c r="F50" s="2"/>
+    </row>
+    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A51" s="2"/>
+      <c r="B51" s="2"/>
+      <c r="C51" s="2"/>
+      <c r="D51" s="2"/>
+      <c r="E51" s="2"/>
+      <c r="F51" s="2"/>
+    </row>
+    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A52" s="2"/>
+      <c r="B52" s="2"/>
+      <c r="C52" s="2"/>
+      <c r="D52" s="2"/>
+      <c r="E52" s="2"/>
+      <c r="F52" s="2"/>
+    </row>
+    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A53" s="2"/>
+      <c r="B53" s="2"/>
+      <c r="C53" s="2"/>
+      <c r="D53" s="2"/>
+      <c r="E53" s="2"/>
+      <c r="F53" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
fixed bug where user is correct while saying too few animals
</commit_message>
<xml_diff>
--- a/test_cases.xlsx
+++ b/test_cases.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="28908"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="29005"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="18180" windowHeight="26740" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Show" sheetId="1" r:id="rId1"/>
@@ -479,9 +479,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J56"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E20" sqref="E20:E21"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -529,6 +527,7 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -547,6 +546,7 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -599,7 +599,7 @@
       </c>
       <c r="E6" s="3"/>
       <c r="F6" s="2"/>
-      <c r="G6" s="5"/>
+      <c r="G6" s="4"/>
       <c r="H6" s="5"/>
       <c r="I6" s="5"/>
       <c r="J6" s="5"/>
@@ -621,7 +621,7 @@
       <c r="F7" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -641,7 +641,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -661,7 +661,7 @@
       </c>
       <c r="E9" s="3"/>
       <c r="F9" s="2"/>
-      <c r="G9" s="5"/>
+      <c r="G9" s="4"/>
       <c r="H9" s="5"/>
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
@@ -681,7 +681,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -701,7 +701,7 @@
       </c>
       <c r="E11" s="3"/>
       <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -807,7 +807,7 @@
       </c>
       <c r="E16" s="3"/>
       <c r="F16" s="2"/>
-      <c r="G16" s="5"/>
+      <c r="G16" s="4"/>
       <c r="H16" s="5"/>
       <c r="I16" s="5"/>
       <c r="J16" s="5"/>
@@ -827,7 +827,7 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -867,7 +867,7 @@
       </c>
       <c r="E19" s="3"/>
       <c r="F19" s="2"/>
-      <c r="G19" s="5"/>
+      <c r="G19" s="4"/>
       <c r="H19" s="5"/>
       <c r="I19" s="5"/>
       <c r="J19" s="5"/>
@@ -959,6 +959,7 @@
       </c>
       <c r="E24" s="3"/>
       <c r="F24" s="2"/>
+      <c r="G24" s="2"/>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A25" s="2" t="s">
@@ -1023,6 +1024,7 @@
       </c>
       <c r="E28" s="3"/>
       <c r="F28" s="2"/>
+      <c r="G28" s="2"/>
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A29" s="2" t="s">
@@ -1053,6 +1055,7 @@
       </c>
       <c r="E30" s="3"/>
       <c r="F30" s="2"/>
+      <c r="G30" s="2"/>
     </row>
     <row r="31" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A31" s="2"/>
@@ -1271,9 +1274,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J53"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E24" sqref="E24:E26"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1321,6 +1322,7 @@
       <c r="F2" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G2" s="2"/>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="2" t="s">
@@ -1339,6 +1341,7 @@
       <c r="F3" s="2" t="s">
         <v>8</v>
       </c>
+      <c r="G3" s="2"/>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="2" t="s">
@@ -1411,7 +1414,7 @@
       </c>
       <c r="E7" s="3"/>
       <c r="F7" s="2"/>
-      <c r="G7" s="5"/>
+      <c r="G7" s="4"/>
       <c r="H7" s="5"/>
       <c r="I7" s="5"/>
       <c r="J7" s="5"/>
@@ -1431,7 +1434,7 @@
       </c>
       <c r="E8" s="3"/>
       <c r="F8" s="2"/>
-      <c r="G8" s="5"/>
+      <c r="G8" s="4"/>
       <c r="H8" s="5"/>
       <c r="I8" s="5"/>
       <c r="J8" s="5"/>
@@ -1471,7 +1474,7 @@
       </c>
       <c r="E10" s="3"/>
       <c r="F10" s="2"/>
-      <c r="G10" s="5"/>
+      <c r="G10" s="4"/>
       <c r="H10" s="5"/>
       <c r="I10" s="5"/>
       <c r="J10" s="5"/>
@@ -1493,7 +1496,7 @@
         <v>29</v>
       </c>
       <c r="F11" s="2"/>
-      <c r="G11" s="5"/>
+      <c r="G11" s="4"/>
       <c r="H11" s="5"/>
       <c r="I11" s="5"/>
       <c r="J11" s="5"/>
@@ -1555,7 +1558,7 @@
       </c>
       <c r="E14" s="3"/>
       <c r="F14" s="2"/>
-      <c r="G14" s="5"/>
+      <c r="G14" s="4"/>
       <c r="H14" s="5"/>
       <c r="I14" s="5"/>
       <c r="J14" s="5"/>
@@ -1575,7 +1578,7 @@
       </c>
       <c r="E15" s="3"/>
       <c r="F15" s="2"/>
-      <c r="G15" s="5"/>
+      <c r="G15" s="4"/>
       <c r="H15" s="5"/>
       <c r="I15" s="5"/>
       <c r="J15" s="5"/>
@@ -1615,7 +1618,7 @@
       </c>
       <c r="E17" s="3"/>
       <c r="F17" s="2"/>
-      <c r="G17" s="5"/>
+      <c r="G17" s="4"/>
       <c r="H17" s="5"/>
       <c r="I17" s="5"/>
       <c r="J17" s="5"/>
@@ -1691,6 +1694,7 @@
       </c>
       <c r="E21" s="3"/>
       <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A22" s="2" t="s">
@@ -1707,6 +1711,7 @@
       </c>
       <c r="E22" s="3"/>
       <c r="F22" s="2"/>
+      <c r="G22" s="2"/>
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A23" s="2" t="s">
@@ -1755,6 +1760,7 @@
       </c>
       <c r="E25" s="3"/>
       <c r="F25" s="2"/>
+      <c r="G25" s="2"/>
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">

</xml_diff>